<commit_message>
refs #649 Auswertung fertig
</commit_message>
<xml_diff>
--- a/doc/Bericht/05_Technischer Bericht/03_Vorstudie/Passantenanalyse.xlsx
+++ b/doc/Bericht/05_Technischer Bericht/03_Vorstudie/Passantenanalyse.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="904" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="904" uniqueCount="190">
   <si>
     <t>Zeit</t>
   </si>
@@ -280,9 +280,6 @@
   </si>
   <si>
     <t>3-7</t>
-  </si>
-  <si>
-    <t>34</t>
   </si>
   <si>
     <t>7-8</t>
@@ -943,8 +940,8 @@
   <dimension ref="A1:Q549"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D267" sqref="D267"/>
+      <pane ySplit="1" topLeftCell="A172" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K177" sqref="K177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3202,18 +3199,18 @@
     </row>
     <row r="186" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B186">
         <v>1</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>88</v>
+        <v>30</v>
       </c>
     </row>
     <row r="187" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B187">
         <v>1</v>
@@ -3224,40 +3221,40 @@
     </row>
     <row r="188" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B188">
         <v>1</v>
       </c>
       <c r="C188" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="189" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B189">
         <v>1</v>
       </c>
       <c r="C189" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="190" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B190">
         <v>2</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="191" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B191">
         <v>1</v>
@@ -3268,7 +3265,7 @@
     </row>
     <row r="192" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B192">
         <v>1</v>
@@ -3279,7 +3276,7 @@
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B193">
         <v>5</v>
@@ -3290,18 +3287,18 @@
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B194">
         <v>1</v>
       </c>
       <c r="C194" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B195">
         <v>3</v>
@@ -3312,7 +3309,7 @@
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B196">
         <v>2</v>
@@ -3323,7 +3320,7 @@
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B197">
         <v>2</v>
@@ -3334,7 +3331,7 @@
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B198">
         <v>2</v>
@@ -3345,7 +3342,7 @@
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B199">
         <v>2</v>
@@ -3356,29 +3353,29 @@
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B200">
         <v>3</v>
       </c>
       <c r="C200" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B201">
         <v>2</v>
       </c>
       <c r="C201" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B202">
         <v>2</v>
@@ -3389,7 +3386,7 @@
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B203">
         <v>1</v>
@@ -3400,7 +3397,7 @@
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B204">
         <v>1</v>
@@ -3411,7 +3408,7 @@
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B205">
         <v>1</v>
@@ -3422,7 +3419,7 @@
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B206">
         <v>1</v>
@@ -3433,7 +3430,7 @@
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B207">
         <v>1</v>
@@ -3444,7 +3441,7 @@
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B208">
         <v>1</v>
@@ -3455,7 +3452,7 @@
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B209">
         <v>2</v>
@@ -3466,18 +3463,18 @@
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B210">
+        <v>1</v>
+      </c>
+      <c r="C210" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="B210">
-        <v>1</v>
-      </c>
-      <c r="C210" s="2" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B211">
         <v>1</v>
@@ -3488,7 +3485,7 @@
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B212">
         <v>1</v>
@@ -3499,7 +3496,7 @@
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B213">
         <v>1</v>
@@ -3510,7 +3507,7 @@
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B214">
         <v>5</v>
@@ -3521,7 +3518,7 @@
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B215">
         <v>4</v>
@@ -3532,7 +3529,7 @@
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B216">
         <v>3</v>
@@ -3543,7 +3540,7 @@
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B217">
         <v>2</v>
@@ -3554,7 +3551,7 @@
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B218">
         <v>3</v>
@@ -3565,7 +3562,7 @@
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B219">
         <v>1</v>
@@ -3576,7 +3573,7 @@
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B220">
         <v>1</v>
@@ -3587,7 +3584,7 @@
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B221">
         <v>1</v>
@@ -3598,29 +3595,29 @@
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B222">
         <v>5</v>
       </c>
       <c r="C222" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B223">
+        <v>2</v>
+      </c>
+      <c r="C223" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="B223">
-        <v>2</v>
-      </c>
-      <c r="C223" s="2" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B224">
         <v>4</v>
@@ -3631,7 +3628,7 @@
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B225">
         <v>1</v>
@@ -3642,7 +3639,7 @@
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B226">
         <v>1</v>
@@ -3653,7 +3650,7 @@
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B227">
         <v>4</v>
@@ -3664,7 +3661,7 @@
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B228">
         <v>2</v>
@@ -3675,7 +3672,7 @@
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B229">
         <v>3</v>
@@ -3686,7 +3683,7 @@
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B230">
         <v>2</v>
@@ -3697,7 +3694,7 @@
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B231">
         <v>1</v>
@@ -3708,7 +3705,7 @@
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B232">
         <v>1</v>
@@ -3719,7 +3716,7 @@
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B233">
         <v>2</v>
@@ -3730,7 +3727,7 @@
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B234">
         <v>4</v>
@@ -3741,7 +3738,7 @@
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A235" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B235">
         <v>5</v>
@@ -3752,7 +3749,7 @@
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B236">
         <v>1</v>
@@ -3763,7 +3760,7 @@
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A237" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B237">
         <v>4</v>
@@ -3774,7 +3771,7 @@
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B238">
         <v>2</v>
@@ -3785,7 +3782,7 @@
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A239" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B239">
         <v>2</v>
@@ -3796,7 +3793,7 @@
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A240" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B240">
         <v>2</v>
@@ -3807,7 +3804,7 @@
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B241">
         <v>1</v>
@@ -3818,7 +3815,7 @@
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B242">
         <v>2</v>
@@ -3829,7 +3826,7 @@
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A243" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B243">
         <v>1</v>
@@ -3840,7 +3837,7 @@
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A244" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B244">
         <v>1</v>
@@ -3851,7 +3848,7 @@
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B245">
         <v>2</v>
@@ -3862,7 +3859,7 @@
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B246">
         <v>1</v>
@@ -3873,7 +3870,7 @@
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B247">
         <v>2</v>
@@ -3884,7 +3881,7 @@
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B248">
         <v>1</v>
@@ -3895,7 +3892,7 @@
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A249" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B249">
         <v>1</v>
@@ -3906,7 +3903,7 @@
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B250">
         <v>3</v>
@@ -3917,7 +3914,7 @@
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B251">
         <v>3</v>
@@ -3928,7 +3925,7 @@
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B252">
         <v>2</v>
@@ -3939,7 +3936,7 @@
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B253">
         <v>2</v>
@@ -3950,7 +3947,7 @@
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A254" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B254">
         <v>4</v>
@@ -3961,7 +3958,7 @@
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A255" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B255">
         <v>2</v>
@@ -3972,7 +3969,7 @@
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A256" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B256">
         <v>4</v>
@@ -3983,7 +3980,7 @@
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A257" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B257">
         <v>1</v>
@@ -3994,18 +3991,18 @@
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A258" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B258">
+        <v>3</v>
+      </c>
+      <c r="C258" s="2" t="s">
         <v>114</v>
-      </c>
-      <c r="B258">
-        <v>3</v>
-      </c>
-      <c r="C258" s="2" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A259" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B259">
         <v>1</v>
@@ -4016,7 +4013,7 @@
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B260">
         <v>2</v>
@@ -4027,7 +4024,7 @@
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A261" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B261">
         <v>2</v>
@@ -4038,7 +4035,7 @@
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A262" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B262">
         <v>3</v>
@@ -4049,7 +4046,7 @@
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A263" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B263">
         <v>1</v>
@@ -4060,7 +4057,7 @@
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A264" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B264">
         <v>2</v>
@@ -4071,7 +4068,7 @@
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A265" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B265">
         <v>1</v>
@@ -4082,18 +4079,18 @@
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B266">
+        <v>3</v>
+      </c>
+      <c r="C266" s="2" t="s">
         <v>117</v>
-      </c>
-      <c r="B266">
-        <v>3</v>
-      </c>
-      <c r="C266" s="2" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B267">
         <v>10</v>
@@ -4104,29 +4101,29 @@
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B268">
         <v>2</v>
       </c>
       <c r="C268" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A269" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B269">
         <v>2</v>
       </c>
       <c r="C269" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A270" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B270">
         <v>1</v>
@@ -4137,7 +4134,7 @@
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A271" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B271">
         <v>3</v>
@@ -4148,7 +4145,7 @@
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A272" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B272">
         <v>2</v>
@@ -4159,7 +4156,7 @@
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A273" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B273">
         <v>1</v>
@@ -4170,7 +4167,7 @@
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A274" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B274">
         <v>1</v>
@@ -4181,7 +4178,7 @@
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A275" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B275">
         <v>3</v>
@@ -4192,7 +4189,7 @@
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A276" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B276">
         <v>1</v>
@@ -4203,7 +4200,7 @@
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A277" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B277">
         <v>2</v>
@@ -4214,7 +4211,7 @@
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A278" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B278">
         <v>3</v>
@@ -4225,7 +4222,7 @@
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A279" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B279">
         <v>4</v>
@@ -4236,7 +4233,7 @@
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A280" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B280">
         <v>3</v>
@@ -4247,7 +4244,7 @@
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A281" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B281">
         <v>3</v>
@@ -4258,7 +4255,7 @@
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A282" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B282">
         <v>2</v>
@@ -4269,7 +4266,7 @@
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A283" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B283">
         <v>1</v>
@@ -4280,7 +4277,7 @@
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A284" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B284">
         <v>3</v>
@@ -4291,7 +4288,7 @@
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A285" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B285">
         <v>1</v>
@@ -4302,7 +4299,7 @@
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A286" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B286">
         <v>1</v>
@@ -4313,7 +4310,7 @@
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A287" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B287">
         <v>1</v>
@@ -4324,7 +4321,7 @@
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A288" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B288">
         <v>1</v>
@@ -4335,7 +4332,7 @@
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A289" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B289">
         <v>1</v>
@@ -4346,7 +4343,7 @@
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A290" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B290">
         <v>2</v>
@@ -4357,7 +4354,7 @@
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A291" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B291">
         <v>3</v>
@@ -4368,7 +4365,7 @@
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A292" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B292">
         <v>1</v>
@@ -4379,7 +4376,7 @@
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A293" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B293">
         <v>2</v>
@@ -4390,7 +4387,7 @@
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A294" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B294">
         <v>2</v>
@@ -4401,7 +4398,7 @@
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A295" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B295">
         <v>1</v>
@@ -4412,7 +4409,7 @@
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A296" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B296">
         <v>1</v>
@@ -4423,7 +4420,7 @@
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A297" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B297">
         <v>2</v>
@@ -4434,7 +4431,7 @@
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A298" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B298">
         <v>3</v>
@@ -4445,18 +4442,18 @@
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A299" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B299">
+        <v>2</v>
+      </c>
+      <c r="C299" s="2" t="s">
         <v>125</v>
-      </c>
-      <c r="B299">
-        <v>2</v>
-      </c>
-      <c r="C299" s="2" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A300" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B300">
         <v>2</v>
@@ -4464,7 +4461,7 @@
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A301" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B301">
         <v>1</v>
@@ -4472,7 +4469,7 @@
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A302" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B302">
         <v>15</v>
@@ -4480,7 +4477,7 @@
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A303" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B303">
         <v>4</v>
@@ -4488,7 +4485,7 @@
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A304" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B304">
         <v>2</v>
@@ -4496,7 +4493,7 @@
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A305" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B305">
         <v>8</v>
@@ -4504,7 +4501,7 @@
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A306" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B306">
         <v>4</v>
@@ -4512,7 +4509,7 @@
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A307" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B307">
         <v>2</v>
@@ -4520,7 +4517,7 @@
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A308" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B308">
         <v>2</v>
@@ -4528,7 +4525,7 @@
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A309" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B309">
         <v>11</v>
@@ -4536,7 +4533,7 @@
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A310" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B310">
         <v>5</v>
@@ -4544,7 +4541,7 @@
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A311" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B311">
         <v>4</v>
@@ -4552,7 +4549,7 @@
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A312" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B312">
         <v>7</v>
@@ -4560,7 +4557,7 @@
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A313" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B313">
         <v>4</v>
@@ -4568,7 +4565,7 @@
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A314" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B314">
         <v>1</v>
@@ -4576,7 +4573,7 @@
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A315" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B315">
         <v>5</v>
@@ -4584,7 +4581,7 @@
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A316" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B316">
         <v>10</v>
@@ -4592,7 +4589,7 @@
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A317" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B317">
         <v>11</v>
@@ -4600,7 +4597,7 @@
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A318" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B318">
         <v>8</v>
@@ -4608,7 +4605,7 @@
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A319" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B319">
         <v>3</v>
@@ -4616,7 +4613,7 @@
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A320" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B320">
         <v>1</v>
@@ -4624,7 +4621,7 @@
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A321" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B321">
         <v>3</v>
@@ -4632,7 +4629,7 @@
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A322" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B322">
         <v>23</v>
@@ -4640,7 +4637,7 @@
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A323" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B323">
         <v>1</v>
@@ -4648,7 +4645,7 @@
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A324" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B324">
         <v>2</v>
@@ -4656,7 +4653,7 @@
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A325" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B325">
         <v>1</v>
@@ -4664,7 +4661,7 @@
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A326" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B326">
         <v>8</v>
@@ -4672,7 +4669,7 @@
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A327" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B327">
         <v>3</v>
@@ -4680,7 +4677,7 @@
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A328" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B328">
         <v>12</v>
@@ -4688,7 +4685,7 @@
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A329" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B329">
         <v>2</v>
@@ -4696,7 +4693,7 @@
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A330" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B330">
         <v>3</v>
@@ -4704,7 +4701,7 @@
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A331" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B331">
         <v>13</v>
@@ -4712,7 +4709,7 @@
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A332" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B332">
         <v>3</v>
@@ -4720,7 +4717,7 @@
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A333" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B333">
         <v>4</v>
@@ -4728,7 +4725,7 @@
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A334" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B334">
         <v>3</v>
@@ -4736,7 +4733,7 @@
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A335" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B335">
         <v>1</v>
@@ -4744,7 +4741,7 @@
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A336" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B336">
         <v>5</v>
@@ -4752,7 +4749,7 @@
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A337" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B337">
         <v>4</v>
@@ -4760,7 +4757,7 @@
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A338" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B338">
         <v>1</v>
@@ -4768,7 +4765,7 @@
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A339" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B339">
         <v>4</v>
@@ -4776,7 +4773,7 @@
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A340" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B340">
         <v>9</v>
@@ -4784,7 +4781,7 @@
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A341" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B341">
         <v>4</v>
@@ -4792,7 +4789,7 @@
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A342" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B342">
         <v>2</v>
@@ -4800,7 +4797,7 @@
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A343" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B343">
         <v>4</v>
@@ -4808,7 +4805,7 @@
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A344" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B344">
         <v>1</v>
@@ -4816,7 +4813,7 @@
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A345" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B345">
         <v>5</v>
@@ -4824,7 +4821,7 @@
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A346" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B346">
         <v>2</v>
@@ -4832,7 +4829,7 @@
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A347" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B347">
         <v>5</v>
@@ -4840,7 +4837,7 @@
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A348" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B348">
         <v>4</v>
@@ -4848,7 +4845,7 @@
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A349" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B349">
         <v>7</v>
@@ -4856,7 +4853,7 @@
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A350" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B350">
         <v>3</v>
@@ -4864,7 +4861,7 @@
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A351" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B351">
         <v>2</v>
@@ -4872,7 +4869,7 @@
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A352" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B352">
         <v>5</v>
@@ -4880,7 +4877,7 @@
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A353" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B353">
         <v>6</v>
@@ -4888,7 +4885,7 @@
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A354" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B354">
         <v>10</v>
@@ -4896,7 +4893,7 @@
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A355" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B355">
         <v>3</v>
@@ -4904,7 +4901,7 @@
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A356" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B356">
         <v>2</v>
@@ -4912,7 +4909,7 @@
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A357" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B357">
         <v>3</v>
@@ -4920,7 +4917,7 @@
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A358" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B358">
         <v>3</v>
@@ -4928,7 +4925,7 @@
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A359" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B359">
         <v>1</v>
@@ -4936,7 +4933,7 @@
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A360" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B360">
         <v>4</v>
@@ -4944,7 +4941,7 @@
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A361" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B361">
         <v>1</v>
@@ -4952,7 +4949,7 @@
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A362" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B362">
         <v>4</v>
@@ -4960,7 +4957,7 @@
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A363" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B363">
         <v>6</v>
@@ -4968,7 +4965,7 @@
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A364" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B364">
         <v>4</v>
@@ -4976,7 +4973,7 @@
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A365" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B365">
         <v>6</v>
@@ -4984,7 +4981,7 @@
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A366" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B366">
         <v>3</v>
@@ -4992,7 +4989,7 @@
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A367" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B367">
         <v>1</v>
@@ -5000,7 +4997,7 @@
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A368" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B368">
         <v>1</v>
@@ -5008,7 +5005,7 @@
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A369" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B369">
         <v>4</v>
@@ -5016,7 +5013,7 @@
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A370" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B370">
         <v>4</v>
@@ -5024,7 +5021,7 @@
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A371" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B371">
         <v>6</v>
@@ -5032,7 +5029,7 @@
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A372" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B372">
         <v>1</v>
@@ -5040,7 +5037,7 @@
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A373" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B373">
         <v>2</v>
@@ -5048,7 +5045,7 @@
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A374" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B374">
         <v>7</v>
@@ -5056,7 +5053,7 @@
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A375" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B375">
         <v>1</v>
@@ -5064,7 +5061,7 @@
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A376" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B376">
         <v>7</v>
@@ -5072,7 +5069,7 @@
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A377" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B377">
         <v>1</v>
@@ -5080,7 +5077,7 @@
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A378" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B378">
         <v>5</v>
@@ -5088,7 +5085,7 @@
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A379" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B379">
         <v>4</v>
@@ -5096,7 +5093,7 @@
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A380" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B380">
         <v>2</v>
@@ -5104,7 +5101,7 @@
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A381" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B381">
         <v>8</v>
@@ -5112,7 +5109,7 @@
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A382" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B382">
         <v>10</v>
@@ -5120,7 +5117,7 @@
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A383" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B383">
         <v>3</v>
@@ -5128,7 +5125,7 @@
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A384" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B384">
         <v>3</v>
@@ -5136,7 +5133,7 @@
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A385" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B385">
         <v>1</v>
@@ -5144,7 +5141,7 @@
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A386" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B386">
         <v>9</v>
@@ -5152,7 +5149,7 @@
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A387" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B387">
         <v>4</v>
@@ -5160,7 +5157,7 @@
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A388" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B388">
         <v>4</v>
@@ -5168,7 +5165,7 @@
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A389" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B389">
         <v>3</v>
@@ -5176,7 +5173,7 @@
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A390" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B390">
         <v>3</v>
@@ -5184,7 +5181,7 @@
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A391" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B391">
         <v>1</v>
@@ -5192,7 +5189,7 @@
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A392" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B392">
         <v>1</v>
@@ -5200,7 +5197,7 @@
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A393" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B393">
         <v>6</v>
@@ -5208,7 +5205,7 @@
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A394" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B394">
         <v>1</v>
@@ -5216,7 +5213,7 @@
     </row>
     <row r="395" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A395" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B395">
         <v>2</v>
@@ -5224,7 +5221,7 @@
     </row>
     <row r="396" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A396" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B396">
         <v>5</v>
@@ -5232,7 +5229,7 @@
     </row>
     <row r="397" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A397" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B397">
         <v>3</v>
@@ -5240,7 +5237,7 @@
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A398" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B398">
         <v>12</v>
@@ -5248,7 +5245,7 @@
     </row>
     <row r="399" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A399" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B399">
         <v>2</v>
@@ -5256,7 +5253,7 @@
     </row>
     <row r="400" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A400" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B400">
         <v>3</v>
@@ -5264,7 +5261,7 @@
     </row>
     <row r="401" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A401" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B401">
         <v>6</v>
@@ -5272,7 +5269,7 @@
     </row>
     <row r="402" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A402" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B402">
         <v>8</v>
@@ -5280,7 +5277,7 @@
     </row>
     <row r="403" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A403" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B403">
         <v>4</v>
@@ -5288,7 +5285,7 @@
     </row>
     <row r="404" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A404" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B404">
         <v>5</v>
@@ -5296,7 +5293,7 @@
     </row>
     <row r="405" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A405" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B405">
         <v>6</v>
@@ -5304,7 +5301,7 @@
     </row>
     <row r="406" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A406" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B406">
         <v>4</v>
@@ -5312,7 +5309,7 @@
     </row>
     <row r="407" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A407" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B407">
         <v>7</v>
@@ -5320,7 +5317,7 @@
     </row>
     <row r="408" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A408" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B408">
         <v>2</v>
@@ -5328,7 +5325,7 @@
     </row>
     <row r="409" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A409" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B409">
         <v>1</v>
@@ -5336,7 +5333,7 @@
     </row>
     <row r="410" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A410" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B410">
         <v>2</v>
@@ -5344,7 +5341,7 @@
     </row>
     <row r="411" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A411" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B411">
         <v>2</v>
@@ -5352,7 +5349,7 @@
     </row>
     <row r="412" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A412" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B412">
         <v>7</v>
@@ -5360,7 +5357,7 @@
     </row>
     <row r="413" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A413" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B413">
         <v>4</v>
@@ -5368,7 +5365,7 @@
     </row>
     <row r="414" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A414" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B414">
         <v>11</v>
@@ -5376,7 +5373,7 @@
     </row>
     <row r="415" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A415" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B415">
         <v>1</v>
@@ -5384,7 +5381,7 @@
     </row>
     <row r="416" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A416" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B416">
         <v>5</v>
@@ -5392,7 +5389,7 @@
     </row>
     <row r="417" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A417" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B417">
         <v>7</v>
@@ -5400,7 +5397,7 @@
     </row>
     <row r="418" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A418" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B418">
         <v>5</v>
@@ -5408,7 +5405,7 @@
     </row>
     <row r="419" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A419" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B419">
         <v>2</v>
@@ -5416,7 +5413,7 @@
     </row>
     <row r="420" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A420" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B420">
         <v>2</v>
@@ -5424,7 +5421,7 @@
     </row>
     <row r="421" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A421" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B421">
         <v>4</v>
@@ -5432,7 +5429,7 @@
     </row>
     <row r="422" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A422" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B422">
         <v>5</v>
@@ -5440,7 +5437,7 @@
     </row>
     <row r="423" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A423" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B423">
         <v>3</v>
@@ -5448,7 +5445,7 @@
     </row>
     <row r="424" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A424" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B424">
         <v>4</v>
@@ -5456,7 +5453,7 @@
     </row>
     <row r="425" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A425" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B425">
         <v>3</v>
@@ -5464,7 +5461,7 @@
     </row>
     <row r="426" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A426" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B426">
         <v>2</v>
@@ -5472,7 +5469,7 @@
     </row>
     <row r="427" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A427" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B427">
         <v>9</v>
@@ -5480,7 +5477,7 @@
     </row>
     <row r="428" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A428" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B428">
         <v>4</v>
@@ -5488,7 +5485,7 @@
     </row>
     <row r="429" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A429" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B429">
         <v>7</v>
@@ -5496,7 +5493,7 @@
     </row>
     <row r="430" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A430" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B430">
         <v>3</v>
@@ -5504,7 +5501,7 @@
     </row>
     <row r="431" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A431" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B431">
         <v>2</v>
@@ -5512,7 +5509,7 @@
     </row>
     <row r="432" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A432" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B432">
         <v>4</v>
@@ -5520,7 +5517,7 @@
     </row>
     <row r="433" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A433" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B433">
         <v>1</v>
@@ -5528,7 +5525,7 @@
     </row>
     <row r="434" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A434" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B434">
         <v>5</v>
@@ -5536,7 +5533,7 @@
     </row>
     <row r="435" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A435" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B435">
         <v>5</v>
@@ -5544,7 +5541,7 @@
     </row>
     <row r="436" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A436" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B436">
         <v>1</v>
@@ -5552,7 +5549,7 @@
     </row>
     <row r="437" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A437" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B437">
         <v>2</v>
@@ -5560,7 +5557,7 @@
     </row>
     <row r="438" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A438" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B438">
         <v>2</v>
@@ -5568,7 +5565,7 @@
     </row>
     <row r="439" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A439" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B439">
         <v>2</v>
@@ -5576,7 +5573,7 @@
     </row>
     <row r="440" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A440" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B440">
         <v>4</v>
@@ -5584,7 +5581,7 @@
     </row>
     <row r="441" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A441" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B441">
         <v>1</v>
@@ -5592,7 +5589,7 @@
     </row>
     <row r="442" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A442" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B442">
         <v>3</v>
@@ -5600,7 +5597,7 @@
     </row>
     <row r="443" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A443" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B443">
         <v>10</v>
@@ -5608,7 +5605,7 @@
     </row>
     <row r="444" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A444" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B444">
         <v>2</v>
@@ -5616,7 +5613,7 @@
     </row>
     <row r="445" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A445" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B445">
         <v>3</v>
@@ -5624,7 +5621,7 @@
     </row>
     <row r="446" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A446" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B446">
         <v>8</v>
@@ -5632,7 +5629,7 @@
     </row>
     <row r="447" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A447" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B447">
         <v>1</v>
@@ -5640,7 +5637,7 @@
     </row>
     <row r="448" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A448" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B448">
         <v>1</v>
@@ -5648,7 +5645,7 @@
     </row>
     <row r="449" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A449" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B449">
         <v>3</v>
@@ -5656,7 +5653,7 @@
     </row>
     <row r="450" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A450" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B450">
         <v>4</v>
@@ -5664,7 +5661,7 @@
     </row>
     <row r="451" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A451" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B451">
         <v>1</v>
@@ -5672,7 +5669,7 @@
     </row>
     <row r="452" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A452" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B452">
         <v>2</v>
@@ -5680,7 +5677,7 @@
     </row>
     <row r="453" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A453" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B453">
         <v>39</v>
@@ -5688,7 +5685,7 @@
     </row>
     <row r="454" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A454" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B454">
         <v>2</v>
@@ -5696,7 +5693,7 @@
     </row>
     <row r="455" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A455" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B455">
         <v>5</v>
@@ -5704,7 +5701,7 @@
     </row>
     <row r="456" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A456" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B456">
         <v>8</v>
@@ -5712,7 +5709,7 @@
     </row>
     <row r="457" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A457" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B457">
         <v>1</v>
@@ -5720,7 +5717,7 @@
     </row>
     <row r="458" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A458" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B458">
         <v>1</v>
@@ -5728,7 +5725,7 @@
     </row>
     <row r="459" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A459" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B459">
         <v>3</v>
@@ -5736,7 +5733,7 @@
     </row>
     <row r="460" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A460" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B460">
         <v>1</v>
@@ -5744,7 +5741,7 @@
     </row>
     <row r="461" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A461" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B461">
         <v>6</v>
@@ -5752,7 +5749,7 @@
     </row>
     <row r="462" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A462" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B462">
         <v>3</v>
@@ -5760,7 +5757,7 @@
     </row>
     <row r="463" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A463" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B463">
         <v>4</v>
@@ -5768,7 +5765,7 @@
     </row>
     <row r="464" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A464" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B464">
         <v>1</v>
@@ -5776,7 +5773,7 @@
     </row>
     <row r="465" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A465" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B465">
         <v>1</v>
@@ -5784,7 +5781,7 @@
     </row>
     <row r="466" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A466" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B466">
         <v>2</v>
@@ -5792,7 +5789,7 @@
     </row>
     <row r="467" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A467" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B467">
         <v>6</v>
@@ -5800,7 +5797,7 @@
     </row>
     <row r="468" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A468" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B468">
         <v>4</v>
@@ -5808,7 +5805,7 @@
     </row>
     <row r="469" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A469" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B469">
         <v>5</v>
@@ -5816,7 +5813,7 @@
     </row>
     <row r="470" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A470" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B470">
         <v>4</v>
@@ -5824,7 +5821,7 @@
     </row>
     <row r="471" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A471" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B471">
         <v>5</v>
@@ -5832,7 +5829,7 @@
     </row>
     <row r="472" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A472" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B472">
         <v>7</v>
@@ -5840,7 +5837,7 @@
     </row>
     <row r="473" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A473" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B473">
         <v>4</v>
@@ -5848,7 +5845,7 @@
     </row>
     <row r="474" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A474" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B474">
         <v>4</v>
@@ -5856,7 +5853,7 @@
     </row>
     <row r="475" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A475" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B475">
         <v>8</v>
@@ -5864,7 +5861,7 @@
     </row>
     <row r="476" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A476" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B476">
         <v>1</v>
@@ -5872,7 +5869,7 @@
     </row>
     <row r="477" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A477" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B477">
         <v>1</v>
@@ -5880,7 +5877,7 @@
     </row>
     <row r="478" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A478" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B478">
         <v>6</v>
@@ -5888,7 +5885,7 @@
     </row>
     <row r="479" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A479" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B479">
         <v>6</v>
@@ -5896,7 +5893,7 @@
     </row>
     <row r="480" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A480" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B480">
         <v>1</v>
@@ -5904,7 +5901,7 @@
     </row>
     <row r="481" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A481" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B481">
         <v>2</v>
@@ -5912,7 +5909,7 @@
     </row>
     <row r="482" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A482" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B482">
         <v>1</v>
@@ -5920,7 +5917,7 @@
     </row>
     <row r="483" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A483" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B483">
         <v>5</v>
@@ -5928,7 +5925,7 @@
     </row>
     <row r="484" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A484" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B484">
         <v>6</v>
@@ -5936,7 +5933,7 @@
     </row>
     <row r="485" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A485" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B485">
         <v>2</v>
@@ -5944,7 +5941,7 @@
     </row>
     <row r="486" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A486" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B486">
         <v>1</v>
@@ -5952,7 +5949,7 @@
     </row>
     <row r="487" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A487" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B487">
         <v>1</v>
@@ -5960,7 +5957,7 @@
     </row>
     <row r="488" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A488" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B488">
         <v>2</v>
@@ -5968,7 +5965,7 @@
     </row>
     <row r="489" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A489" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B489">
         <v>1</v>
@@ -5976,7 +5973,7 @@
     </row>
     <row r="490" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A490" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B490">
         <v>4</v>
@@ -5984,7 +5981,7 @@
     </row>
     <row r="491" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A491" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B491">
         <v>1</v>
@@ -5992,7 +5989,7 @@
     </row>
     <row r="492" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A492" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B492">
         <v>3</v>
@@ -6000,7 +5997,7 @@
     </row>
     <row r="493" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A493" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B493">
         <v>6</v>
@@ -6008,7 +6005,7 @@
     </row>
     <row r="494" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A494" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B494">
         <v>4</v>
@@ -6016,7 +6013,7 @@
     </row>
     <row r="495" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A495" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B495">
         <v>1</v>
@@ -6024,7 +6021,7 @@
     </row>
     <row r="496" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A496" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B496">
         <v>1</v>
@@ -6032,7 +6029,7 @@
     </row>
     <row r="497" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A497" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B497">
         <v>2</v>
@@ -6040,7 +6037,7 @@
     </row>
     <row r="498" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A498" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B498">
         <v>3</v>
@@ -6048,7 +6045,7 @@
     </row>
     <row r="499" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A499" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B499">
         <v>4</v>
@@ -6056,7 +6053,7 @@
     </row>
     <row r="500" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A500" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B500">
         <v>3</v>
@@ -6064,7 +6061,7 @@
     </row>
     <row r="501" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A501" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B501">
         <v>1</v>
@@ -6072,7 +6069,7 @@
     </row>
     <row r="502" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A502" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B502">
         <v>2</v>
@@ -6080,7 +6077,7 @@
     </row>
     <row r="503" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A503" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B503">
         <v>3</v>
@@ -6088,7 +6085,7 @@
     </row>
     <row r="504" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A504" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B504">
         <v>3</v>
@@ -6096,7 +6093,7 @@
     </row>
     <row r="505" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A505" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B505">
         <v>1</v>
@@ -6104,7 +6101,7 @@
     </row>
     <row r="506" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A506" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B506">
         <v>1</v>
@@ -6112,7 +6109,7 @@
     </row>
     <row r="507" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A507" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B507">
         <v>1</v>
@@ -6120,7 +6117,7 @@
     </row>
     <row r="508" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A508" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B508">
         <v>5</v>
@@ -6128,7 +6125,7 @@
     </row>
     <row r="509" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A509" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B509">
         <v>9</v>
@@ -6136,7 +6133,7 @@
     </row>
     <row r="510" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A510" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B510">
         <v>1</v>
@@ -6144,7 +6141,7 @@
     </row>
     <row r="511" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A511" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B511">
         <v>1</v>
@@ -6152,7 +6149,7 @@
     </row>
     <row r="512" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A512" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B512">
         <v>2</v>
@@ -6160,7 +6157,7 @@
     </row>
     <row r="513" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A513" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B513">
         <v>2</v>
@@ -6168,7 +6165,7 @@
     </row>
     <row r="514" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A514" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B514">
         <v>1</v>
@@ -6176,7 +6173,7 @@
     </row>
     <row r="515" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A515" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B515">
         <v>2</v>
@@ -6184,7 +6181,7 @@
     </row>
     <row r="516" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A516" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B516">
         <v>1</v>
@@ -6192,7 +6189,7 @@
     </row>
     <row r="517" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A517" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B517">
         <v>1</v>
@@ -6200,7 +6197,7 @@
     </row>
     <row r="518" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A518" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B518">
         <v>1</v>
@@ -6208,7 +6205,7 @@
     </row>
     <row r="519" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A519" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B519">
         <v>4</v>
@@ -6216,7 +6213,7 @@
     </row>
     <row r="520" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A520" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B520">
         <v>1</v>
@@ -6224,7 +6221,7 @@
     </row>
     <row r="521" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A521" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B521">
         <v>4</v>
@@ -6232,7 +6229,7 @@
     </row>
     <row r="522" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A522" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B522">
         <v>2</v>
@@ -6240,7 +6237,7 @@
     </row>
     <row r="523" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A523" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B523">
         <v>2</v>
@@ -6248,7 +6245,7 @@
     </row>
     <row r="524" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A524" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B524">
         <v>1</v>
@@ -6256,7 +6253,7 @@
     </row>
     <row r="525" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A525" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B525">
         <v>1</v>
@@ -6264,7 +6261,7 @@
     </row>
     <row r="526" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A526" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B526">
         <v>2</v>
@@ -6272,7 +6269,7 @@
     </row>
     <row r="527" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A527" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B527">
         <v>2</v>
@@ -6280,7 +6277,7 @@
     </row>
     <row r="528" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A528" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B528">
         <v>1</v>
@@ -6288,7 +6285,7 @@
     </row>
     <row r="529" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A529" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B529">
         <v>2</v>
@@ -6296,7 +6293,7 @@
     </row>
     <row r="530" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A530" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B530">
         <v>4</v>
@@ -6304,7 +6301,7 @@
     </row>
     <row r="531" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A531" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B531">
         <v>1</v>
@@ -6312,7 +6309,7 @@
     </row>
     <row r="532" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A532" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B532">
         <v>1</v>
@@ -6320,7 +6317,7 @@
     </row>
     <row r="533" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A533" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B533">
         <v>1</v>
@@ -6328,7 +6325,7 @@
     </row>
     <row r="534" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A534" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B534">
         <v>8</v>
@@ -6336,7 +6333,7 @@
     </row>
     <row r="535" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A535" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B535">
         <v>4</v>
@@ -6344,7 +6341,7 @@
     </row>
     <row r="536" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A536" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B536">
         <v>1</v>
@@ -6352,7 +6349,7 @@
     </row>
     <row r="537" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A537" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B537">
         <v>1</v>
@@ -6360,7 +6357,7 @@
     </row>
     <row r="538" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A538" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B538">
         <v>1</v>
@@ -6368,7 +6365,7 @@
     </row>
     <row r="539" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A539" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B539">
         <v>1</v>
@@ -6376,7 +6373,7 @@
     </row>
     <row r="540" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A540" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B540">
         <v>1</v>
@@ -6384,7 +6381,7 @@
     </row>
     <row r="541" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A541" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B541">
         <v>1</v>
@@ -6392,7 +6389,7 @@
     </row>
     <row r="542" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A542" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B542">
         <v>3</v>
@@ -6400,7 +6397,7 @@
     </row>
     <row r="543" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A543" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B543">
         <v>1</v>
@@ -6408,7 +6405,7 @@
     </row>
     <row r="544" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A544" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B544">
         <v>1</v>
@@ -6416,7 +6413,7 @@
     </row>
     <row r="545" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A545" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B545">
         <v>4</v>
@@ -6424,7 +6421,7 @@
     </row>
     <row r="546" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A546" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B546">
         <v>1</v>
@@ -6432,7 +6429,7 @@
     </row>
     <row r="547" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A547" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B547">
         <v>1</v>
@@ -6440,7 +6437,7 @@
     </row>
     <row r="548" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A548" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B548">
         <v>2</v>
@@ -6448,7 +6445,7 @@
     </row>
     <row r="549" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A549" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B549">
         <v>3</v>

</xml_diff>